<commit_message>
request use permission field is changed to permission with sleightly different explanation
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7DE00B-B659-E645-9502-B08AD92F3270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29FC942-1226-A14A-9F64-78A228D5F7D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,16 +44,81 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    In onze vorige bespreking (11/11/2020), bespraken we dat dit veld ook gebruikt kan worden als filter. Als we nog geen use permission voor materialen hebben, zorgt Martijn er voor dat die materialen nog niet zichtbaar zijn voor end users. Dat is een mooie oplossing, maar het past bij nader inzien niet bij het origineel bedoelde gebruik van dit veld (zie de beschrijving in het gele veld). Om de filter-optie te kunnen gebruiken, moeten we dit veld anders gaan benaderen.
-Voorstel: hernoem veld "Use permission" en maak nieuwe beschrijving voor dit veld: "If we have use permission, select 'yes' from the drop-down menu. If we do not have use permission, select 'no' from the drop-down menu. If we do not have use permission but should obtain permission, select 'no - request use permission' from the drop-down menu." Martijn, je kunt beide 'no' opties eruit filteren, zodat ze niet zichtbaar zijn voor end users, toch?</t>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    In onze vorige bespreking (11/11/2020), bespraken we dat dit veld ook gebruikt kan worden als filter. Als we nog geen use permission voor materialen hebben, zorgt Martijn er voor dat die materialen nog niet zichtbaar zijn voor end users. Dat is een mooie oplossing, maar het past bij nader inzien niet bij het origineel bedoelde gebruik van dit veld (zie de beschrijving in het gele veld). Om de filter-optie te kunnen gebruiken, moeten we dit veld anders gaan benaderen.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Voorstel: hernoem veld "Use permission" en maak nieuwe beschrijving voor dit veld: "If we have use permission, select 'yes' from the drop-down menu. If we do not have use permission, select 'no' from the drop-down menu. If we do not have use permission but should obtain permission, select 'no - request use permission' from the drop-down menu." Martijn, je kunt beide 'no' opties eruit filteren, zodat ze niet zichtbaar zijn voor end users, toch?</t>
         </r>
       </text>
     </comment>
@@ -90,15 +155,61 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Als we de mogelijkheid tot image upload toevoegen, moeten we ook een veld met use permission toevoegen, niet?</t>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Als we de mogelijkheid tot image upload toevoegen, moeten we ook een veld met use permission toevoegen, niet?</t>
         </r>
       </text>
     </comment>
@@ -180,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="189">
   <si>
     <t>Field</t>
   </si>
@@ -295,9 +406,6 @@
 c. If it is available on our own website, select 'available on site' from the menu.</t>
   </si>
   <si>
-    <t>Request Use Permission</t>
-  </si>
-  <si>
     <t>Rated</t>
   </si>
   <si>
@@ -315,9 +423,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>This is a reminder for the research group. If you do not have use permission yet, but want to request it, indicate that here (‘Yes’), so that you can later follow up on it. If you fill in ‘No’ here, it will be assumed that the material can be used freely.</t>
   </si>
   <si>
     <t>Film</t>
@@ -451,9 +556,6 @@
   </si>
   <si>
     <t>Date released</t>
-  </si>
-  <si>
-    <t>Request use permission</t>
   </si>
   <si>
     <t>thumbnail</t>
@@ -756,9 +858,6 @@
     <t>Be concise and type a description of max. 500 characters here. Please deliver a description of the image (both literal imagery and potential deeper meaning). If needed, include important and/or noteworthy information on the material that is not yet mentioned in other parts of your entry.</t>
   </si>
   <si>
-    <t>This is a reminder for the research group. If you do not have use permission for the image of the person yet, but want to request it, indicate that here (‘Yes’), so that you can later follow up on it. If you fill in ‘No’ here, it will be assumed that the material can be used freely.</t>
-  </si>
-  <si>
     <t>Indicate when the material was released. If you do not have a date (for example, because the music was not released on an album), look at the description (on YouTube or other platform) for a release or perfomance date . If it is not included, use the upload date. Use one of the following formats:
 Day: 1999-12-04 (Y-M-D)
 b. Month: 1999-12 (Y-M)
@@ -890,6 +989,15 @@
 To add a new location:
 Type the name of the location. This can be a village, town, city, region, country, continent etc. 
  If after adding the location, you still cannot find the specific location, report the issue to Martijn Bentum on Github.</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Permission</t>
+  </si>
+  <si>
+    <t>If you have permission to use the materials indicate yes, if you intend to request permission indicate 'request use permission' otherwise indicate no</t>
   </si>
 </sst>
 </file>
@@ -1401,17 +1509,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -1452,57 +1560,57 @@
     </row>
     <row r="2" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1514,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1683,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1586,7 +1694,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1594,10 +1702,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1608,7 +1716,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1619,7 +1727,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -1641,7 +1749,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1652,7 +1760,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1671,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>19</v>
@@ -1685,7 +1793,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1696,7 +1804,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -1707,7 +1815,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="144" x14ac:dyDescent="0.2">
@@ -1715,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>23</v>
@@ -1726,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>24</v>
@@ -1752,7 +1860,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -1782,10 +1890,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -1793,10 +1901,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -1804,10 +1912,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1815,10 +1923,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1826,10 +1934,10 @@
         <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1843,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1865,7 +1973,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1876,10 +1984,10 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -1887,7 +1995,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1898,161 +2006,161 @@
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>25</v>
@@ -2063,29 +2171,29 @@
     </row>
     <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>30</v>
@@ -2096,57 +2204,57 @@
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2158,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2180,7 +2288,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2191,10 +2299,10 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -2202,7 +2310,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -2213,76 +2321,76 @@
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -2290,18 +2398,18 @@
     </row>
     <row r="12" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
@@ -2312,18 +2420,18 @@
     </row>
     <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -2334,7 +2442,7 @@
     </row>
     <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -2345,57 +2453,57 @@
     </row>
     <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2407,8 +2515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2429,7 +2537,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2440,10 +2548,10 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -2451,7 +2559,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -2462,87 +2570,87 @@
     </row>
     <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>23</v>
@@ -2550,18 +2658,18 @@
     </row>
     <row r="13" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
@@ -2572,18 +2680,18 @@
     </row>
     <row r="15" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>28</v>
@@ -2594,7 +2702,7 @@
     </row>
     <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
@@ -2605,57 +2713,57 @@
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2667,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2689,7 +2797,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2700,10 +2808,10 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -2711,7 +2819,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -2722,98 +2830,98 @@
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>23</v>
@@ -2821,18 +2929,18 @@
     </row>
     <row r="14" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
@@ -2843,29 +2951,29 @@
     </row>
     <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -2876,57 +2984,57 @@
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2939,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2961,7 +3069,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2972,10 +3080,10 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -2983,7 +3091,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -2994,120 +3102,120 @@
     </row>
     <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="C13" s="14" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>23</v>
@@ -3115,10 +3223,10 @@
     </row>
     <row r="16" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
@@ -3126,7 +3234,7 @@
     </row>
     <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
@@ -3137,29 +3245,29 @@
     </row>
     <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>30</v>
@@ -3170,57 +3278,57 @@
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3232,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3254,157 +3362,157 @@
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3440,90 +3548,90 @@
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C6" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added protocal text person thumbnail
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29FC942-1226-A14A-9F64-78A228D5F7D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8000E89E-F7F0-534E-9FBD-9F45466D5BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -889,9 +889,6 @@
     <t xml:space="preserve">Upload a thumbnail of the material here of max. 400x400 pixels (or about 300kb); this will be displayed alongside the entry in the repository. </t>
   </si>
   <si>
-    <t xml:space="preserve">Upload a thumbnail of the image of the person here of max. 400x400 pixels (or about 300kb); this will be displayed alongside the entry in the repository. </t>
-  </si>
-  <si>
     <t>Direct your queries and questions about working with this repository to Lindsay Janssen: l.janssen@let.ru.nl</t>
   </si>
   <si>
@@ -998,6 +995,9 @@
   </si>
   <si>
     <t>If you have permission to use the materials indicate yes, if you intend to request permission indicate 'request use permission' otherwise indicate no</t>
+  </si>
+  <si>
+    <t>Upload a thumbnail of the image of the person here of max. 400X400 pixels (or about 300kb); this will be displayed alongside the entry in the repository. Only upload an image here if you have use permission for that image; if this is not the case, do not upload anything.</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="4" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -1538,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1566,7 +1566,7 @@
         <v>129</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1588,7 +1588,7 @@
         <v>131</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
         <v>132</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1683,7 +1683,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1705,7 +1705,7 @@
         <v>152</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1749,7 +1749,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1760,7 +1760,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1815,7 +1815,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="144" x14ac:dyDescent="0.2">
@@ -1890,10 +1890,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -2012,7 +2012,7 @@
         <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2056,7 +2056,7 @@
         <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -2067,7 +2067,7 @@
         <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2111,7 +2111,7 @@
         <v>155</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2207,10 +2207,10 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2327,7 +2327,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2360,7 +2360,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -2371,7 +2371,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2382,7 +2382,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2456,10 +2456,10 @@
         <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
         <v>93</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2620,7 +2620,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -2631,7 +2631,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2642,7 +2642,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2716,10 +2716,10 @@
         <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
         <v>98</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2987,10 +2987,10 @@
         <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3108,7 +3108,7 @@
         <v>112</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3152,7 +3152,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3163,7 +3163,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3185,7 +3185,7 @@
         <v>87</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -3207,7 +3207,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -3281,10 +3281,10 @@
         <v>111</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3340,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3412,7 +3412,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -3423,7 +3423,7 @@
         <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -3437,7 +3437,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>157</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3456,7 +3456,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -3500,7 +3500,7 @@
         <v>83</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -3509,10 +3509,10 @@
         <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3565,7 +3565,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -3576,7 +3576,7 @@
         <v>124</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3598,7 +3598,7 @@
         <v>125</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added protocol changed permission for the different sources models
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8000E89E-F7F0-534E-9FBD-9F45466D5BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98CC320-CD03-FA49-B9FD-F78E435B2F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -994,10 +994,10 @@
     <t xml:space="preserve"> Permission</t>
   </si>
   <si>
-    <t>If you have permission to use the materials indicate yes, if you intend to request permission indicate 'request use permission' otherwise indicate no</t>
-  </si>
-  <si>
     <t>Upload a thumbnail of the image of the person here of max. 400X400 pixels (or about 300kb); this will be displayed alongside the entry in the repository. Only upload an image here if you have use permission for that image; if this is not the case, do not upload anything.</t>
+  </si>
+  <si>
+    <t>If you have permission to use the material, indicate "yes"; if you intend to request use permission, indicate "request use permission"; otherwise indicate "no". Only materials for which you indicated you have use permission will be made available to end users; other materials will remain invisible for end users.</t>
   </si>
 </sst>
 </file>
@@ -1885,7 +1885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>5</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>185</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -2202,7 +2202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>185</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2451,7 +2451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>83</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>185</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2711,7 +2711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>92</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>185</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2982,7 +2982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>185</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3047,7 +3047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3276,7 +3276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>111</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>185</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3340,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3445,7 +3445,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>186</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added protocol for person pseudonym
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98CC320-CD03-FA49-B9FD-F78E435B2F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A307F00D-6B9A-6F41-B4BB-1AE30AF6A70D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -133,7 +133,7 @@
     <author>tc={CC94FBC0-0FAC-47EF-A7C6-3205BC49AD30}</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{F7DBCE83-71A1-4035-AF36-C51DDD929C84}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{F7DBCE83-71A1-4035-AF36-C51DDD929C84}">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="1" shapeId="0" xr:uid="{CC94FBC0-0FAC-47EF-A7C6-3205BC49AD30}">
+    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{CC94FBC0-0FAC-47EF-A7C6-3205BC49AD30}">
       <text>
         <r>
           <rPr>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="191">
   <si>
     <t>Field</t>
   </si>
@@ -998,6 +998,12 @@
   </si>
   <si>
     <t>If you have permission to use the material, indicate "yes"; if you intend to request use permission, indicate "request use permission"; otherwise indicate "no". Only materials for which you indicated you have use permission will be made available to end users; other materials will remain invisible for end users.</t>
+  </si>
+  <si>
+    <t>Pseudonym</t>
+  </si>
+  <si>
+    <t>Enter one or more pseudonyms seperated by a comma e.g. George Sand, Aurore</t>
   </si>
 </sst>
 </file>
@@ -3047,7 +3053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3338,10 +3344,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3376,21 +3382,21 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3398,21 +3404,21 @@
         <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>178</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -3420,54 +3426,54 @@
         <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -3475,43 +3481,54 @@
         <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="15" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>188</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed protocol text to include video game model and setting field
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CDC789-4D81-E249-8AEC-C3463825607B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26022194-BA68-1C48-9919-4C11BE3148D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="Picturestory" sheetId="8" r:id="rId7"/>
     <sheet name="Person" sheetId="2" r:id="rId8"/>
     <sheet name="Keyword" sheetId="11" r:id="rId9"/>
-    <sheet name="Famine" sheetId="9" r:id="rId10"/>
-    <sheet name="Location" sheetId="10" r:id="rId11"/>
+    <sheet name="Videogame" sheetId="12" r:id="rId10"/>
+    <sheet name="Famine" sheetId="9" r:id="rId11"/>
+    <sheet name="Location" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -292,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="219">
   <si>
     <t>Field</t>
   </si>
@@ -950,9 +951,6 @@
 - 'could not load the results': this means the server could not complete the request, the locations could be in the database.</t>
   </si>
   <si>
-    <t>Select a text type from the drop-down menu. You can select one film type.  If your film can be labelled as different film types, select the most representative option, and, optionally, add other film types in the description field. If your film type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
-  </si>
-  <si>
     <t>First make sure the location you want to add is not in the database. You can enter the name in a location field (e.g in the add film form). If this shows the message:  'no results found', the location is not in the database. You can also check whether the location is in the database under view (top of your window) go to location and search for the location you want to add.
 To add a new location:
 Type the name of the location. This can be a village, town, city, region, country, continent etc. 
@@ -1038,13 +1036,67 @@
   </si>
   <si>
     <t>If this keyword belongs to a category, please select the category keyword below</t>
+  </si>
+  <si>
+    <t>Game type</t>
+  </si>
+  <si>
+    <t>Select a game type from the drop-down menu. You can select one game type.  If your videogame can be labelled as different game types, select the most representative option, and, optionally, add other game types in the description field. If your game type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
+  </si>
+  <si>
+    <t>Production studio</t>
+  </si>
+  <si>
+    <t>Select the production studio from the drop-down menu. If the studio is not yet included, add the studio to the list.  You can do so by clicking on the plus sign right next to the production studio field.</t>
+  </si>
+  <si>
+    <t>If you can provide a link to the game, include that here.</t>
+  </si>
+  <si>
+    <t>Videogame</t>
+  </si>
+  <si>
+    <t>Select the location the game is situated</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>What is the original language, or are the original languages of the game?  You can select multiple languages.</t>
+  </si>
+  <si>
+    <t>Include a link to official information about the film here (the game's website, the production studio's website, for example).</t>
+  </si>
+  <si>
+    <t>Person who created this short movie e.g. news reports, amateur reports, etc.</t>
+  </si>
+  <si>
+    <t>Select the location the text is situated</t>
+  </si>
+  <si>
+    <t>Select the location the film is situated</t>
+  </si>
+  <si>
+    <t>Select the location the image is situated</t>
+  </si>
+  <si>
+    <t>Select a film type from the drop-down menu. You can select one film type.  If your film can be labelled as different film types, select the most representative option, and, optionally, add other film types in the description field. If your film type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
+  </si>
+  <si>
+    <t>Select the location the infographic is about</t>
+  </si>
+  <si>
+    <t>Select the location the music is about</t>
+  </si>
+  <si>
+    <t>Select the location the picture story  is situated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1096,6 +1148,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1130,7 +1189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1189,6 +1248,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1578,6 +1643,267 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4D6185-2899-B648-9CFC-43E1146B32C0}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1695,7 +2021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1727,7 +2053,7 @@
         <v>127</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1779,10 +2105,10 @@
         <v>126</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1792,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1822,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1833,7 +2159,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1965,7 +2291,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -1976,7 +2302,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -2062,10 +2388,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -2109,7 +2435,18 @@
         <v>87</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2121,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2151,7 +2488,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2162,7 +2499,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2184,7 +2521,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>173</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2198,70 +2535,70 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2269,32 +2606,32 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2302,21 +2639,21 @@
         <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2324,109 +2661,131 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>182</v>
+      <c r="C28" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2436,10 +2795,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2466,7 +2825,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2477,7 +2836,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2543,7 +2902,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2628,10 +2987,10 @@
         <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2675,7 +3034,18 @@
         <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2685,10 +3055,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2715,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2726,7 +3096,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2803,7 +3173,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2888,10 +3258,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2935,7 +3305,18 @@
         <v>87</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2945,10 +3326,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2975,7 +3356,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2986,7 +3367,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3159,10 +3540,10 @@
         <v>95</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3206,7 +3587,18 @@
         <v>68</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3217,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3247,7 +3639,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3258,7 +3650,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3357,7 +3749,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="128" x14ac:dyDescent="0.2">
@@ -3368,7 +3760,7 @@
         <v>112</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -3453,10 +3845,10 @@
         <v>109</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3500,7 +3892,18 @@
         <v>87</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3548,10 +3951,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3628,7 +4031,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3692,10 +4095,10 @@
         <v>38</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>176</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3707,10 +4110,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9952C2-DAA8-8841-9400-1BE8DA0F0498}">
-  <dimension ref="A20:C23"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3719,48 +4122,48 @@
     <col min="3" max="3" width="88" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="5" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#66 added model recorded speech with simple models recordedspeech_type and broadcastStation, created form and list view and added protocol text; signal util backup function now includes a try except clause to be able to add new models
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26022194-BA68-1C48-9919-4C11BE3148D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765991E-CE6E-BA49-82AB-AEB1AF327216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="Person" sheetId="2" r:id="rId8"/>
     <sheet name="Keyword" sheetId="11" r:id="rId9"/>
     <sheet name="Videogame" sheetId="12" r:id="rId10"/>
-    <sheet name="Famine" sheetId="9" r:id="rId11"/>
-    <sheet name="Location" sheetId="10" r:id="rId12"/>
+    <sheet name="Recordedspeech" sheetId="13" r:id="rId11"/>
+    <sheet name="Famine" sheetId="9" r:id="rId12"/>
+    <sheet name="Location" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -293,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="231">
   <si>
     <t>Field</t>
   </si>
@@ -1065,9 +1066,6 @@
     <t>What is the original language, or are the original languages of the game?  You can select multiple languages.</t>
   </si>
   <si>
-    <t>Include a link to official information about the film here (the game's website, the production studio's website, for example).</t>
-  </si>
-  <si>
     <t>Person who created this short movie e.g. news reports, amateur reports, etc.</t>
   </si>
   <si>
@@ -1090,6 +1088,45 @@
   </si>
   <si>
     <t>Select the location the picture story  is situated</t>
+  </si>
+  <si>
+    <t>Recordedspeech</t>
+  </si>
+  <si>
+    <t>Speech type</t>
+  </si>
+  <si>
+    <t>Broadcasting station</t>
+  </si>
+  <si>
+    <t>Audio link</t>
+  </si>
+  <si>
+    <t>Select the location speech is situated</t>
+  </si>
+  <si>
+    <t>Include a link to official information about the video game here (the game's website, the production studio's website, for example).</t>
+  </si>
+  <si>
+    <t>Select a speech type from the drop-down menu. You can select one speech type.  If your speech type can be labelled as different speech types, select the most representative option, and, optionally, add other speech types in the description field. If your speech type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
+  </si>
+  <si>
+    <t>Select the broadcasting station from the drop-down menu. If the station is not yet included, add the station to the list.  You can do so by clicking on the plus sign right next to the broadcasting station field.</t>
+  </si>
+  <si>
+    <t>Include a link to official information about the speech here ( the broadcasting station's website, for example).</t>
+  </si>
+  <si>
+    <t>If you can provide a link to the recording, include that here.</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persons who created this recording </t>
+  </si>
+  <si>
+    <t>Persons speaking during the recording</t>
   </si>
 </sst>
 </file>
@@ -1646,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4D6185-2899-B648-9CFC-43E1146B32C0}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1741,7 +1778,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1904,6 +1941,279 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712FB1F3-5B74-2C4C-BD15-5A7ABF9FB5C1}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2021,7 +2331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2446,7 +2756,7 @@
         <v>208</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2460,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:C29"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2521,7 +2831,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2543,7 +2853,7 @@
         <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2785,7 +3095,7 @@
         <v>208</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3355,7 @@
         <v>208</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3316,7 +3626,7 @@
         <v>208</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3598,7 +3908,7 @@
         <v>208</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3903,7 +4213,7 @@
         <v>208</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#67 added memorial site form and list view with related model memorial site type
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765991E-CE6E-BA49-82AB-AEB1AF327216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F295401-8616-E943-9B21-66698FD04CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -24,8 +24,9 @@
     <sheet name="Keyword" sheetId="11" r:id="rId9"/>
     <sheet name="Videogame" sheetId="12" r:id="rId10"/>
     <sheet name="Recordedspeech" sheetId="13" r:id="rId11"/>
-    <sheet name="Famine" sheetId="9" r:id="rId12"/>
-    <sheet name="Location" sheetId="10" r:id="rId13"/>
+    <sheet name="Memorialsite" sheetId="14" r:id="rId12"/>
+    <sheet name="Famine" sheetId="9" r:id="rId13"/>
+    <sheet name="Location" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -294,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="244">
   <si>
     <t>Field</t>
   </si>
@@ -1126,7 +1127,46 @@
     <t xml:space="preserve">Persons who created this recording </t>
   </si>
   <si>
-    <t>Persons speaking during the recording</t>
+    <t>Persons speaking during this recording</t>
+  </si>
+  <si>
+    <t>Locations recorded</t>
+  </si>
+  <si>
+    <t>The location this recording is recorded</t>
+  </si>
+  <si>
+    <t>memorialsite</t>
+  </si>
+  <si>
+    <t>Memorial type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persons who created this memorial site </t>
+  </si>
+  <si>
+    <t>Persons who designed this memorial site</t>
+  </si>
+  <si>
+    <t>The location(s) of the memorial site</t>
+  </si>
+  <si>
+    <t>Select the location memorial is about</t>
+  </si>
+  <si>
+    <t>Include a link to official information about the memorial site</t>
+  </si>
+  <si>
+    <t>If you can provide a link to the video recording of the memorial site</t>
+  </si>
+  <si>
+    <t>Select a memorial type from the drop-down menu. You can select one memorial type.  If your memorial type can be labelled as different memorial types, select the most representative option, and, optionally, add other memorial types in the description field. If your memorial type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
+  </si>
+  <si>
+    <t>Donors</t>
+  </si>
+  <si>
+    <t>Persons who financially contributed to the memorial site</t>
   </si>
 </sst>
 </file>
@@ -1942,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712FB1F3-5B74-2C4C-BD15-5A7ABF9FB5C1}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2048,142 +2088,142 @@
         <v>218</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>221</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>118</v>
+        <v>87</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2191,20 +2231,31 @@
         <v>218</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2214,6 +2265,289 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA195A6-50F4-0041-9BCC-1DD91B5730EF}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="120.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2331,7 +2665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3107,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed some protocol texts
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F295401-8616-E943-9B21-66698FD04CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D975B9F-C99F-B74D-872C-57A3A89E9FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="246">
   <si>
     <t>Field</t>
   </si>
@@ -1025,9 +1025,6 @@
     <t>If you consider the item an important piece (key piece) which should feature prominently in the repository, click on the flag to make it red.</t>
   </si>
   <si>
-    <t>Enter one or more pseudonyms separated by a comma e.g. George Sand, Aurore</t>
-  </si>
-  <si>
     <t>Keyword</t>
   </si>
   <si>
@@ -1167,6 +1164,15 @@
   </si>
   <si>
     <t>Persons who financially contributed to the memorial site</t>
+  </si>
+  <si>
+    <t>Enter one or more pseudonyms separated by a comma e.g. George Sand, Aurore (check the box if the pseudonym should take precedent over the real name)</t>
+  </si>
+  <si>
+    <t>If you have an image file, upload that here. Use of .jpg files is strongly preferred; only use another format if it is not possible to upload the image as a .jpg file. Use a file which is as small as possible without quality loss. Before uploading the file, name the file in the following format: "last name creator_first 3 or 4 words of title.jpg". So, for example, for Salvador Dali's painting The Persistence of Memory: "dali_thepersistenceofmemory.jpg". If the creator is anonymous, use "anon". If the image does not have an official title, use 3 of 4 words that describe the image. So for an uncredited and/or untitled photograph of women lining up for food stamps: "anon_womenliningup.jpg". If you have more than one image of the same memorial site, serially number your images. So: "dali_thepersistenceofmemory_1.jpg"; "dali_thepersistenceofmemory_2.jpg", etc. If the image can only be accessed through a link, make a screenshot of the image and use that screenshot for own research use. If you indicate “no” or “to request” in the permission field, we as researchers will see the screenshot, but the end users will only have access to the link.</t>
+  </si>
+  <si>
+    <t>What is the original language, or are the original languages of the recorded speech?  You can select multiple languages.</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1741,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1746,7 +1752,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1757,7 +1763,7 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
@@ -1768,7 +1774,7 @@
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1779,73 +1785,73 @@
     </row>
     <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>65</v>
@@ -1856,7 +1862,7 @@
     </row>
     <row r="12" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
@@ -1867,7 +1873,7 @@
     </row>
     <row r="13" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>67</v>
@@ -1878,7 +1884,7 @@
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -1889,7 +1895,7 @@
     </row>
     <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
@@ -1900,7 +1906,7 @@
     </row>
     <row r="16" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -1911,7 +1917,7 @@
     </row>
     <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1922,7 +1928,7 @@
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -1933,7 +1939,7 @@
     </row>
     <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>87</v>
@@ -1944,7 +1950,7 @@
     </row>
     <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
@@ -1955,7 +1961,7 @@
     </row>
     <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
@@ -1966,7 +1972,7 @@
     </row>
     <row r="22" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>174</v>
@@ -1985,7 +1991,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1997,7 +2003,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2008,7 +2014,7 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2019,7 +2025,7 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
@@ -2030,7 +2036,7 @@
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -2041,106 +2047,106 @@
     </row>
     <row r="5" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>66</v>
@@ -2151,7 +2157,7 @@
     </row>
     <row r="15" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>67</v>
@@ -2162,7 +2168,7 @@
     </row>
     <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -2173,7 +2179,7 @@
     </row>
     <row r="17" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
@@ -2184,7 +2190,7 @@
     </row>
     <row r="18" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -2195,7 +2201,7 @@
     </row>
     <row r="19" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
@@ -2206,7 +2212,7 @@
     </row>
     <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>34</v>
@@ -2217,7 +2223,7 @@
     </row>
     <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>87</v>
@@ -2228,7 +2234,7 @@
     </row>
     <row r="22" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
@@ -2239,7 +2245,7 @@
     </row>
     <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
@@ -2250,7 +2256,7 @@
     </row>
     <row r="24" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>174</v>
@@ -2268,7 +2274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA195A6-50F4-0041-9BCC-1DD91B5730EF}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2280,7 +2286,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2291,7 +2297,7 @@
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -2302,7 +2308,7 @@
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
@@ -2313,7 +2319,7 @@
     </row>
     <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -2324,49 +2330,49 @@
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>81</v>
       </c>
@@ -2374,56 +2380,56 @@
         <v>85</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>66</v>
@@ -2434,7 +2440,7 @@
     </row>
     <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>67</v>
@@ -2445,7 +2451,7 @@
     </row>
     <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -2456,7 +2462,7 @@
     </row>
     <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
@@ -2467,7 +2473,7 @@
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -2478,7 +2484,7 @@
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
@@ -2489,7 +2495,7 @@
     </row>
     <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>34</v>
@@ -2500,7 +2506,7 @@
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>87</v>
@@ -2511,7 +2517,7 @@
     </row>
     <row r="22" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
@@ -2522,7 +2528,7 @@
     </row>
     <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
@@ -2533,7 +2539,7 @@
     </row>
     <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>174</v>
@@ -3087,10 +3093,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3105,7 +3111,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3165,7 +3171,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3187,7 +3193,7 @@
         <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3426,10 +3432,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3686,10 +3692,10 @@
         <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3957,10 +3963,10 @@
         <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4239,10 +4245,10 @@
         <v>95</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -4544,10 +4550,10 @@
         <v>109</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4559,8 +4565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4590,7 +4596,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -4598,7 +4604,7 @@
         <v>177</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -4768,18 +4774,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>32</v>
@@ -4790,7 +4796,7 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>34</v>
@@ -4801,13 +4807,13 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added text for donor institutions
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E90B7EF-6EE4-7344-B3A1-A6BC46430D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D30845F-6B64-E84B-ACC5-55B5AF830E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="248">
   <si>
     <t>Field</t>
   </si>
@@ -1154,9 +1154,6 @@
     <t>Select a memorial type from the drop-down menu. You can select one memorial type.  If your memorial type can be labelled as different memorial types, select the most representative option, and, optionally, add other memorial types in the description field. If your memorial type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
   </si>
   <si>
-    <t>Donors</t>
-  </si>
-  <si>
     <t>Persons who financially contributed to the memorial site</t>
   </si>
   <si>
@@ -1173,6 +1170,15 @@
 You might get the following error messages when using the autocomplete field:
 - 'no results found': This means there is no location matching that name.
 - 'could not load the results': this means the server could not complete the request, the locations could be in the database.</t>
+  </si>
+  <si>
+    <t>Donors (person)</t>
+  </si>
+  <si>
+    <t>Donors (institution)</t>
+  </si>
+  <si>
+    <t>Institutions who financially contributed to the memorial site</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2147,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="192" x14ac:dyDescent="0.2">
@@ -2272,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA195A6-50F4-0041-9BCC-1DD91B5730EF}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2295,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>231</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>231</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>231</v>
       </c>
@@ -2366,32 +2372,32 @@
         <v>231</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2399,10 +2405,10 @@
         <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>206</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2410,10 +2416,10 @@
         <v>231</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>237</v>
+        <v>206</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2421,21 +2427,21 @@
         <v>231</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>78</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2443,54 +2449,54 @@
         <v>231</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2498,10 +2504,10 @@
         <v>231</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2509,42 +2515,53 @@
         <v>231</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C25" s="16" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3110,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3226,7 +3243,7 @@
         <v>59</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -4604,7 +4621,7 @@
         <v>176</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#68 added commissioning fields for person and institution and the corresponding protocol text
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D30845F-6B64-E84B-ACC5-55B5AF830E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CF3EF9-DFC1-C048-BB1A-3DFA133464DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="252">
   <si>
     <t>Field</t>
   </si>
@@ -1179,6 +1179,18 @@
   </si>
   <si>
     <t>Institutions who financially contributed to the memorial site</t>
+  </si>
+  <si>
+    <t>Commissioning persons</t>
+  </si>
+  <si>
+    <t>Commissioning institutions</t>
+  </si>
+  <si>
+    <t>Indicate here which person(s)  gave the assignment for the work. If the person, is not yet included, add them using the plus sign next to the 'commissioning ' field.</t>
+  </si>
+  <si>
+    <t>Indicate here which institution(s), or funding body/bodies gave the assignment for the work. If the  institution, or funding body is not yet included, add them using the plus sign next to the 'commissioning' field.</t>
   </si>
 </sst>
 </file>
@@ -2278,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA195A6-50F4-0041-9BCC-1DD91B5730EF}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2389,37 +2401,37 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>231</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>248</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>206</v>
+        <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2427,10 +2439,10 @@
         <v>231</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>237</v>
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2438,87 +2450,87 @@
         <v>231</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>206</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2526,42 +2538,64 @@
         <v>231</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new model Artefact
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CF3EF9-DFC1-C048-BB1A-3DFA133464DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4828F8AA-49FA-4740-9089-94296750D4BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -25,8 +25,9 @@
     <sheet name="Videogame" sheetId="12" r:id="rId10"/>
     <sheet name="Recordedspeech" sheetId="13" r:id="rId11"/>
     <sheet name="Memorialsite" sheetId="14" r:id="rId12"/>
-    <sheet name="Famine" sheetId="9" r:id="rId13"/>
-    <sheet name="Location" sheetId="10" r:id="rId14"/>
+    <sheet name="Artefact" sheetId="15" r:id="rId13"/>
+    <sheet name="Famine" sheetId="9" r:id="rId14"/>
+    <sheet name="Location" sheetId="10" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -295,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="258">
   <si>
     <t>Field</t>
   </si>
@@ -1191,6 +1192,34 @@
   </si>
   <si>
     <t>Indicate here which institution(s), or funding body/bodies gave the assignment for the work. If the  institution, or funding body is not yet included, add them using the plus sign next to the 'commissioning' field.</t>
+  </si>
+  <si>
+    <t>Artefact</t>
+  </si>
+  <si>
+    <t>Artefact type</t>
+  </si>
+  <si>
+    <t>Select an artefact type from the drop-down menu. You can select one artefact type.  If your image can be labelled as different artefact types, select the most representative option, and, optionally, add other artefact types in the description field. If your artefact type is not on the list do not add it, but report this to Lindsay Janssen (l.janssen@let.ru.nl). She will add it.</t>
+  </si>
+  <si>
+    <t>(If not applicable, leave empty.) Indicate when the material was released. Use one of the following formats:
+Day: 1999-12-04 (Y-M-D)
+b. Month: 1999-12 (Y-M)
+c. Year: 1999y (y)
+d. Decade: 200d (d 1990-2000)
+e. Century: 20c (twentieth eentury, or c 1900-2000)
+f. Millenium: 2m (second millenium, or m 1000-2000)
+For date ranges, you are limited to formats d-f above. If you need to be more specific (for example, a series ran from 1941 until 1952), Indicate the final year (1952) here and indicate the full date range in the Description field.</t>
+  </si>
+  <si>
+    <t>Select the location the artefact is situated</t>
+  </si>
+  <si>
+    <t>Indicate here where the material was created. Start typing the placename and then select a location from the auto-fill menu. If your location is not yet on the list, add it via the plus sign right next the Locations field.
+You might get the following error messages when using the autocomplete field:
+- 'no results found': This means there is no location matching that name.
+- 'could not load the results': this means the server could not complete the request, the locations could be in the database.</t>
   </si>
 </sst>
 </file>
@@ -2292,7 +2321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA195A6-50F4-0041-9BCC-1DD91B5730EF}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2605,6 +2634,254 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344F55E-A4D0-6147-A7A7-5F1BCE57AF2B}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2722,7 +2999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3498,8 +3775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added viaf field to persons #89
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4828F8AA-49FA-4740-9089-94296750D4BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E92DA42-69CA-7F4A-BDDE-3440C25E88AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="260">
   <si>
     <t>Field</t>
   </si>
@@ -1220,6 +1220,12 @@
 You might get the following error messages when using the autocomplete field:
 - 'no results found': This means there is no location matching that name.
 - 'could not load the results': this means the server could not complete the request, the locations could be in the database.</t>
+  </si>
+  <si>
+    <t>VIAF</t>
+  </si>
+  <si>
+    <t>You can find the viaf at viaf.org/​</t>
   </si>
 </sst>
 </file>
@@ -2637,7 +2643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8344F55E-A4D0-6147-A7A7-5F1BCE57AF2B}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -4891,10 +4897,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5077,6 +5083,17 @@
       </c>
       <c r="C16" s="16" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed field from person
</commit_message>
<xml_diff>
--- a/data/Protocols.xlsx
+++ b/data/Protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/django/hoh/heritages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E92DA42-69CA-7F4A-BDDE-3440C25E88AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADED0658-CEC2-F447-AD10-FC67994510FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary" sheetId="6" r:id="rId1"/>
@@ -135,7 +135,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F7DBCE83-71A1-4035-AF36-C51DDD929C84}</author>
-    <author>tc={CC94FBC0-0FAC-47EF-A7C6-3205BC49AD30}</author>
   </authors>
   <commentList>
     <comment ref="A15" authorId="0" shapeId="0" xr:uid="{F7DBCE83-71A1-4035-AF36-C51DDD929C84}">
@@ -152,69 +151,6 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is not in the repository (yet)?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{CC94FBC0-0FAC-47EF-A7C6-3205BC49AD30}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Comment:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">    Als we de mogelijkheid tot image upload toevoegen, moeten we ook een veld met use permission toevoegen, niet?</t>
         </r>
       </text>
     </comment>
@@ -296,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="259">
   <si>
     <t>Field</t>
   </si>
@@ -955,9 +891,6 @@
   </si>
   <si>
     <t>Permission</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Permission</t>
   </si>
   <si>
     <t>If you have permission to use the material, indicate "yes"; if you intend to request use permission, indicate "request use permission"; otherwise indicate "no". Only materials for which you indicated you have use permission will be made available to end users; other materials will remain invisible for end users.</t>
@@ -1794,7 +1727,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1805,29 +1738,29 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1838,73 +1771,73 @@
     </row>
     <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>65</v>
@@ -1915,7 +1848,7 @@
     </row>
     <row r="12" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
@@ -1926,7 +1859,7 @@
     </row>
     <row r="13" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>67</v>
@@ -1937,7 +1870,7 @@
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -1948,7 +1881,7 @@
     </row>
     <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
@@ -1959,7 +1892,7 @@
     </row>
     <row r="16" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -1970,7 +1903,7 @@
     </row>
     <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1981,7 +1914,7 @@
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -1992,18 +1925,18 @@
     </row>
     <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
@@ -2014,7 +1947,7 @@
     </row>
     <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
@@ -2025,13 +1958,13 @@
     </row>
     <row r="22" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +1989,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2067,29 +2000,29 @@
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -2100,106 +2033,106 @@
     </row>
     <row r="5" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>66</v>
@@ -2210,7 +2143,7 @@
     </row>
     <row r="15" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>67</v>
@@ -2221,7 +2154,7 @@
     </row>
     <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -2232,7 +2165,7 @@
     </row>
     <row r="17" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
@@ -2243,7 +2176,7 @@
     </row>
     <row r="18" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -2254,7 +2187,7 @@
     </row>
     <row r="19" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
@@ -2265,7 +2198,7 @@
     </row>
     <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>34</v>
@@ -2276,18 +2209,18 @@
     </row>
     <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
@@ -2298,7 +2231,7 @@
     </row>
     <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
@@ -2309,13 +2242,13 @@
     </row>
     <row r="24" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2339,7 +2272,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2350,29 +2283,29 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -2383,79 +2316,79 @@
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="128" x14ac:dyDescent="0.2">
@@ -2466,56 +2399,56 @@
         <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>66</v>
@@ -2526,7 +2459,7 @@
     </row>
     <row r="18" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>67</v>
@@ -2537,7 +2470,7 @@
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -2548,7 +2481,7 @@
     </row>
     <row r="20" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>25</v>
@@ -2559,7 +2492,7 @@
     </row>
     <row r="21" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>30</v>
@@ -2570,7 +2503,7 @@
     </row>
     <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>32</v>
@@ -2581,7 +2514,7 @@
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
@@ -2592,18 +2525,18 @@
     </row>
     <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
@@ -2614,7 +2547,7 @@
     </row>
     <row r="26" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>28</v>
@@ -2625,13 +2558,13 @@
     </row>
     <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2664,29 +2597,29 @@
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -2697,18 +2630,18 @@
     </row>
     <row r="5" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>83</v>
@@ -2719,7 +2652,7 @@
     </row>
     <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>62</v>
@@ -2730,29 +2663,29 @@
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>86</v>
@@ -2763,18 +2696,18 @@
     </row>
     <row r="11" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -2785,7 +2718,7 @@
     </row>
     <row r="13" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
@@ -2796,7 +2729,7 @@
     </row>
     <row r="14" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -2807,7 +2740,7 @@
     </row>
     <row r="15" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -2818,18 +2751,18 @@
     </row>
     <row r="16" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
@@ -2840,7 +2773,7 @@
     </row>
     <row r="18" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>32</v>
@@ -2851,7 +2784,7 @@
     </row>
     <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
@@ -2862,24 +2795,24 @@
     </row>
     <row r="20" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3089,10 +3022,10 @@
         <v>126</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3065,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3143,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3275,7 +3208,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -3286,7 +3219,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -3375,7 +3308,7 @@
         <v>173</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3419,7 +3352,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3427,10 +3360,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3472,7 +3405,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3483,7 +3416,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3505,7 +3438,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3527,7 +3460,7 @@
         <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3560,7 +3493,7 @@
         <v>59</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -3714,7 +3647,7 @@
         <v>173</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3758,7 +3691,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3766,10 +3699,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3809,7 +3742,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3820,7 +3753,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3886,7 +3819,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -3974,7 +3907,7 @@
         <v>173</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -4018,7 +3951,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4026,10 +3959,10 @@
         <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4080,7 +4013,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4157,7 +4090,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -4245,7 +4178,7 @@
         <v>173</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -4289,7 +4222,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4297,10 +4230,10 @@
         <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4273,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4351,7 +4284,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4527,7 +4460,7 @@
         <v>173</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -4571,7 +4504,7 @@
         <v>68</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4579,10 +4512,10 @@
         <v>95</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4623,7 +4556,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4634,7 +4567,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -4733,7 +4666,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="128" x14ac:dyDescent="0.2">
@@ -4744,7 +4677,7 @@
         <v>112</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -4832,7 +4765,7 @@
         <v>173</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -4876,7 +4809,7 @@
         <v>87</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4884,10 +4817,10 @@
         <v>109</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4897,10 +4830,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4935,10 +4868,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5015,7 +4948,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -5074,26 +5007,15 @@
       </c>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -5119,18 +5041,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>32</v>
@@ -5141,7 +5063,7 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>34</v>
@@ -5152,13 +5074,13 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>